<commit_message>
Finished verifying and making notes on current sensors
</commit_message>
<xml_diff>
--- a/Calculations/Sensing/Current_Sense_Amps_Options.xlsx
+++ b/Calculations/Sensing/Current_Sense_Amps_Options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ghani\Documents\ECE Projects\Variable_Voltage_Controller\Calculations\Sensing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7D72A84-BBA4-476C-844A-B1F892E5F07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6E9E92-5F6D-439D-8508-AEF1CD622514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5268C5C5-1FB9-4FB4-9FFF-D1E7639C19CF}"/>
   </bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>